<commit_message>
Take failed screenshot implemented
</commit_message>
<xml_diff>
--- a/src/test/java/com/tmb/dataproviders/inputexcels/HomePageTestDataProvider.xlsx
+++ b/src/test/java/com/tmb/dataproviders/inputexcels/HomePageTestDataProvider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hensi\IdeaProjects\FrameWork1\src\test\java\com\tmb\dataproviders\inputexcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CE7C62-F078-41EA-B4B2-E891AFE0896C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6AC415-8A60-4FC1-8BEC-726C857A0388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -49,9 +49,6 @@
     <t>homepage test2 field 1</t>
   </si>
   <si>
-    <t>homepage test2 field 10</t>
-  </si>
-  <si>
     <t>homepage test1 field 1</t>
   </si>
   <si>
@@ -61,13 +58,10 @@
     <t>homepage test1 field10</t>
   </si>
   <si>
-    <t>homepage test1 field30</t>
-  </si>
-  <si>
     <t>homepage test1 field20</t>
   </si>
   <si>
-    <t>homepage test1 field40</t>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -416,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,10 +443,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -463,24 +457,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -490,10 +470,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E8F295-990B-4D4F-BADD-241A21BE5BFE}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,21 +497,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>